<commit_message>
Update of Logbook and Time Schedule
</commit_message>
<xml_diff>
--- a/Planning/TimeSchedule.xlsx
+++ b/Planning/TimeSchedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Desktop\school\NTU\modules\y4s1\FYP\FYP-IEM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryan\Desktop\school\NTU\modules\y4s1\FYP\FYP-IEM\Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{DB534A89-E2BD-4AFD-8F47-3A9535AD9C06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E87DB2-929D-462C-AA25-09DE84E4F96A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Task 3</t>
   </si>
@@ -248,6 +248,9 @@
   </si>
   <si>
     <t>Building Display</t>
+  </si>
+  <si>
+    <t>Cardboard Prototype</t>
   </si>
 </sst>
 </file>
@@ -828,7 +831,36 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="8" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -841,36 +873,7 @@
     <xf numFmtId="14" fontId="8" fillId="0" borderId="3" xfId="9" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="3" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="4" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="11" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="10" borderId="2" xfId="10" applyNumberFormat="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1128,13 +1131,13 @@
           <xdr:col>4</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>390525</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>9526</xdr:rowOff>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1195,7 +1198,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8638EF3-2DAE-40BC-A45A-2B8C536FAB0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1496,11 +1499,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK35"/>
+  <dimension ref="A1:BK36"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1550,10 +1553,10 @@
         <v>41</v>
       </c>
       <c r="C3" s="62"/>
-      <c r="D3" s="67">
+      <c r="D3" s="76">
         <v>44054</v>
       </c>
-      <c r="E3" s="67"/>
+      <c r="E3" s="76"/>
     </row>
     <row r="4" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
@@ -1563,96 +1566,96 @@
       <c r="D4" s="6">
         <v>1</v>
       </c>
-      <c r="H4" s="64">
+      <c r="H4" s="73">
         <f>H5</f>
         <v>44053</v>
       </c>
-      <c r="I4" s="65"/>
-      <c r="J4" s="65"/>
-      <c r="K4" s="65"/>
-      <c r="L4" s="65"/>
-      <c r="M4" s="65"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="64">
+      <c r="I4" s="74"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="74"/>
+      <c r="N4" s="75"/>
+      <c r="O4" s="73">
         <f>O5</f>
         <v>44060</v>
       </c>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="66"/>
-      <c r="V4" s="64">
+      <c r="P4" s="74"/>
+      <c r="Q4" s="74"/>
+      <c r="R4" s="74"/>
+      <c r="S4" s="74"/>
+      <c r="T4" s="74"/>
+      <c r="U4" s="75"/>
+      <c r="V4" s="73">
         <f>V5</f>
         <v>44067</v>
       </c>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
-      <c r="Y4" s="65"/>
-      <c r="Z4" s="65"/>
-      <c r="AA4" s="65"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="64">
+      <c r="W4" s="74"/>
+      <c r="X4" s="74"/>
+      <c r="Y4" s="74"/>
+      <c r="Z4" s="74"/>
+      <c r="AA4" s="74"/>
+      <c r="AB4" s="75"/>
+      <c r="AC4" s="73">
         <f>AC5</f>
         <v>44074</v>
       </c>
-      <c r="AD4" s="65"/>
-      <c r="AE4" s="65"/>
-      <c r="AF4" s="65"/>
-      <c r="AG4" s="65"/>
-      <c r="AH4" s="65"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="64">
+      <c r="AD4" s="74"/>
+      <c r="AE4" s="74"/>
+      <c r="AF4" s="74"/>
+      <c r="AG4" s="74"/>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="75"/>
+      <c r="AJ4" s="73">
         <f>AJ5</f>
         <v>44081</v>
       </c>
-      <c r="AK4" s="65"/>
-      <c r="AL4" s="65"/>
-      <c r="AM4" s="65"/>
-      <c r="AN4" s="65"/>
-      <c r="AO4" s="65"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="64">
+      <c r="AK4" s="74"/>
+      <c r="AL4" s="74"/>
+      <c r="AM4" s="74"/>
+      <c r="AN4" s="74"/>
+      <c r="AO4" s="74"/>
+      <c r="AP4" s="75"/>
+      <c r="AQ4" s="73">
         <f>AQ5</f>
         <v>44088</v>
       </c>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="65"/>
-      <c r="AT4" s="65"/>
-      <c r="AU4" s="65"/>
-      <c r="AV4" s="65"/>
-      <c r="AW4" s="66"/>
-      <c r="AX4" s="64">
+      <c r="AR4" s="74"/>
+      <c r="AS4" s="74"/>
+      <c r="AT4" s="74"/>
+      <c r="AU4" s="74"/>
+      <c r="AV4" s="74"/>
+      <c r="AW4" s="75"/>
+      <c r="AX4" s="73">
         <f>AX5</f>
         <v>44095</v>
       </c>
-      <c r="AY4" s="65"/>
-      <c r="AZ4" s="65"/>
-      <c r="BA4" s="65"/>
-      <c r="BB4" s="65"/>
-      <c r="BC4" s="65"/>
-      <c r="BD4" s="66"/>
-      <c r="BE4" s="64">
+      <c r="AY4" s="74"/>
+      <c r="AZ4" s="74"/>
+      <c r="BA4" s="74"/>
+      <c r="BB4" s="74"/>
+      <c r="BC4" s="74"/>
+      <c r="BD4" s="75"/>
+      <c r="BE4" s="73">
         <f>BE5</f>
         <v>44102</v>
       </c>
-      <c r="BF4" s="65"/>
-      <c r="BG4" s="65"/>
-      <c r="BH4" s="65"/>
-      <c r="BI4" s="65"/>
-      <c r="BJ4" s="65"/>
-      <c r="BK4" s="66"/>
+      <c r="BF4" s="74"/>
+      <c r="BG4" s="74"/>
+      <c r="BH4" s="74"/>
+      <c r="BI4" s="74"/>
+      <c r="BJ4" s="74"/>
+      <c r="BK4" s="75"/>
     </row>
     <row r="5" spans="1:63" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="77"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="77"/>
       <c r="H5" s="10">
         <f>Project_Start-WEEKDAY(Project_Start,1)+2+7*(Display_Week-1)</f>
         <v>44053</v>
@@ -2201,7 +2204,7 @@
       <c r="E8" s="19"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15" t="str">
-        <f t="shared" ref="G8:G33" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G34" si="6">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H8" s="35"/>
@@ -2269,11 +2272,11 @@
         <v>44</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="D9" s="68">
+      <c r="D9" s="63">
         <f>Project_Start</f>
         <v>44054</v>
       </c>
-      <c r="E9" s="68">
+      <c r="E9" s="63">
         <f>D9+14</f>
         <v>44068</v>
       </c>
@@ -2347,10 +2350,10 @@
         <v>45</v>
       </c>
       <c r="C10" s="20"/>
-      <c r="D10" s="68">
+      <c r="D10" s="63">
         <v>44060</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="63">
         <f>D10+8</f>
         <v>44068</v>
       </c>
@@ -2422,10 +2425,10 @@
         <v>46</v>
       </c>
       <c r="C11" s="20"/>
-      <c r="D11" s="68">
+      <c r="D11" s="63">
         <v>44069</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="63">
         <f>D11+13</f>
         <v>44082</v>
       </c>
@@ -2497,11 +2500,11 @@
         <v>47</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="D12" s="68">
+      <c r="D12" s="63">
         <f>D11+7</f>
         <v>44076</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="63">
         <f>D12+6</f>
         <v>44082</v>
       </c>
@@ -2573,10 +2576,10 @@
         <v>48</v>
       </c>
       <c r="C13" s="20"/>
-      <c r="D13" s="68">
+      <c r="D13" s="63">
         <v>44075</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="63">
         <f>D13+8</f>
         <v>44083</v>
       </c>
@@ -2650,8 +2653,8 @@
         <v>49</v>
       </c>
       <c r="C14" s="22"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="70"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15" t="str">
         <f t="shared" si="6"/>
@@ -2717,21 +2720,18 @@
     <row r="15" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="50"/>
       <c r="B15" s="58" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C15" s="23"/>
-      <c r="D15" s="71">
-        <v>44084</v>
-      </c>
-      <c r="E15" s="71">
-        <f>D15+15</f>
-        <v>44099</v>
+      <c r="D15" s="66">
+        <v>44088</v>
+      </c>
+      <c r="E15" s="66">
+        <f>D15+5</f>
+        <v>44093</v>
       </c>
       <c r="F15" s="15"/>
-      <c r="G15" s="15">
-        <f t="shared" si="6"/>
-        <v>16</v>
-      </c>
+      <c r="G15" s="15"/>
       <c r="H15" s="35"/>
       <c r="I15" s="35"/>
       <c r="J15" s="35"/>
@@ -2790,22 +2790,22 @@
       <c r="BK15" s="35"/>
     </row>
     <row r="16" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
+      <c r="A16" s="50"/>
       <c r="B16" s="58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C16" s="23"/>
-      <c r="D16" s="71">
-        <v>44095</v>
-      </c>
-      <c r="E16" s="71">
-        <f>D16+7</f>
-        <v>44102</v>
+      <c r="D16" s="66">
+        <v>44084</v>
+      </c>
+      <c r="E16" s="66">
+        <f>D16+15</f>
+        <v>44099</v>
       </c>
       <c r="F16" s="15"/>
       <c r="G16" s="15">
         <f t="shared" si="6"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H16" s="35"/>
       <c r="I16" s="35"/>
@@ -2819,8 +2819,8 @@
       <c r="Q16" s="35"/>
       <c r="R16" s="35"/>
       <c r="S16" s="35"/>
-      <c r="T16" s="36"/>
-      <c r="U16" s="36"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
       <c r="V16" s="35"/>
       <c r="W16" s="35"/>
       <c r="X16" s="35"/>
@@ -2867,20 +2867,20 @@
     <row r="17" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="49"/>
       <c r="B17" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C17" s="23"/>
-      <c r="D17" s="71">
+      <c r="D17" s="66">
+        <v>44095</v>
+      </c>
+      <c r="E17" s="66">
+        <f>D17+7</f>
         <v>44102</v>
-      </c>
-      <c r="E17" s="71">
-        <f>D17+21</f>
-        <v>44123</v>
       </c>
       <c r="F17" s="15"/>
       <c r="G17" s="15">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="H17" s="35"/>
       <c r="I17" s="35"/>
@@ -2894,8 +2894,8 @@
       <c r="Q17" s="35"/>
       <c r="R17" s="35"/>
       <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
       <c r="V17" s="35"/>
       <c r="W17" s="35"/>
       <c r="X17" s="35"/>
@@ -2942,21 +2942,20 @@
     <row r="18" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49"/>
       <c r="B18" s="58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="23"/>
-      <c r="D18" s="71">
-        <f>D17+13</f>
-        <v>44115</v>
-      </c>
-      <c r="E18" s="71">
-        <f>D18+14</f>
-        <v>44129</v>
+      <c r="D18" s="66">
+        <v>44102</v>
+      </c>
+      <c r="E18" s="66">
+        <f>D18+21</f>
+        <v>44123</v>
       </c>
       <c r="F18" s="15"/>
       <c r="G18" s="15">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H18" s="35"/>
       <c r="I18" s="35"/>
@@ -2974,7 +2973,7 @@
       <c r="U18" s="35"/>
       <c r="V18" s="35"/>
       <c r="W18" s="35"/>
-      <c r="X18" s="36"/>
+      <c r="X18" s="35"/>
       <c r="Y18" s="35"/>
       <c r="Z18" s="35"/>
       <c r="AA18" s="35"/>
@@ -3015,16 +3014,24 @@
       <c r="BJ18" s="35"/>
       <c r="BK18" s="35"/>
     </row>
-    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49"/>
-      <c r="B19" s="58"/>
+      <c r="B19" s="58" t="s">
+        <v>55</v>
+      </c>
       <c r="C19" s="23"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
+      <c r="D19" s="66">
+        <f>D18+13</f>
+        <v>44115</v>
+      </c>
+      <c r="E19" s="66">
+        <f>D19+14</f>
+        <v>44129</v>
+      </c>
       <c r="F19" s="15"/>
-      <c r="G19" s="15" t="str">
+      <c r="G19" s="15">
         <f t="shared" si="6"/>
-        <v/>
+        <v>15</v>
       </c>
       <c r="H19" s="35"/>
       <c r="I19" s="35"/>
@@ -3042,7 +3049,7 @@
       <c r="U19" s="35"/>
       <c r="V19" s="35"/>
       <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
+      <c r="X19" s="36"/>
       <c r="Y19" s="35"/>
       <c r="Z19" s="35"/>
       <c r="AA19" s="35"/>
@@ -3083,16 +3090,12 @@
       <c r="BJ19" s="35"/>
       <c r="BK19" s="35"/>
     </row>
-    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="73"/>
+    <row r="20" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="49"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15" t="str">
         <f t="shared" si="6"/>
@@ -3156,22 +3159,19 @@
       <c r="BK20" s="35"/>
     </row>
     <row r="21" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="49"/>
-      <c r="B21" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="74">
-        <v>44129</v>
-      </c>
-      <c r="E21" s="74">
-        <f>D21+21</f>
-        <v>44150</v>
-      </c>
+      <c r="A21" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="25"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="68"/>
       <c r="F21" s="15"/>
-      <c r="G21" s="15">
+      <c r="G21" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>22</v>
+        <v/>
       </c>
       <c r="H21" s="35"/>
       <c r="I21" s="35"/>
@@ -3230,18 +3230,23 @@
       <c r="BJ21" s="35"/>
       <c r="BK21" s="35"/>
     </row>
-    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="49"/>
       <c r="B22" s="59" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C22" s="26"/>
-      <c r="D22" s="74"/>
-      <c r="E22" s="74"/>
+      <c r="D22" s="69">
+        <v>44129</v>
+      </c>
+      <c r="E22" s="69">
+        <f>D22+21</f>
+        <v>44150</v>
+      </c>
       <c r="F22" s="15"/>
-      <c r="G22" s="15" t="str">
+      <c r="G22" s="15">
         <f t="shared" si="6"/>
-        <v/>
+        <v>22</v>
       </c>
       <c r="H22" s="35"/>
       <c r="I22" s="35"/>
@@ -3303,11 +3308,11 @@
     <row r="23" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49"/>
       <c r="B23" s="59" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23" s="26"/>
-      <c r="D23" s="74"/>
-      <c r="E23" s="74"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="15"/>
       <c r="G23" s="15" t="str">
         <f t="shared" si="6"/>
@@ -3373,11 +3378,11 @@
     <row r="24" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="49"/>
       <c r="B24" s="59" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24" s="26"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15" t="str">
         <f t="shared" si="6"/>
@@ -3443,11 +3448,11 @@
     <row r="25" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49"/>
       <c r="B25" s="59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="26"/>
-      <c r="D25" s="74"/>
-      <c r="E25" s="74"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15" t="str">
         <f t="shared" si="6"/>
@@ -3510,16 +3515,14 @@
       <c r="BJ25" s="35"/>
       <c r="BK25" s="35"/>
     </row>
-    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="28"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="76"/>
+    <row r="26" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="49"/>
+      <c r="B26" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15" t="str">
         <f t="shared" si="6"/>
@@ -3583,21 +3586,19 @@
       <c r="BK26" s="35"/>
     </row>
     <row r="27" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
-      <c r="B27" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="77">
-        <v>44144</v>
-      </c>
-      <c r="E27" s="77">
-        <v>44148</v>
-      </c>
+      <c r="A27" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="71"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="15">
+      <c r="G27" s="15" t="str">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v/>
       </c>
       <c r="H27" s="35"/>
       <c r="I27" s="35"/>
@@ -3656,22 +3657,22 @@
       <c r="BJ27" s="35"/>
       <c r="BK27" s="35"/>
     </row>
-    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="49"/>
       <c r="B28" s="60" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
       <c r="C28" s="29"/>
-      <c r="D28" s="77" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="77" t="s">
-        <v>26</v>
+      <c r="D28" s="72">
+        <v>44144</v>
+      </c>
+      <c r="E28" s="72">
+        <v>44148</v>
       </c>
       <c r="F28" s="15"/>
-      <c r="G28" s="15" t="e">
+      <c r="G28" s="15">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>5</v>
       </c>
       <c r="H28" s="35"/>
       <c r="I28" s="35"/>
@@ -3733,13 +3734,13 @@
     <row r="29" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
       <c r="B29" s="60" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C29" s="29"/>
-      <c r="D29" s="77" t="s">
+      <c r="D29" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="77" t="s">
+      <c r="E29" s="72" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="15"/>
@@ -3807,13 +3808,13 @@
     <row r="30" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="49"/>
       <c r="B30" s="60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" s="29"/>
-      <c r="D30" s="77" t="s">
+      <c r="D30" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="77" t="s">
+      <c r="E30" s="72" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="15"/>
@@ -3881,13 +3882,13 @@
     <row r="31" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="49"/>
       <c r="B31" s="60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="29"/>
-      <c r="D31" s="77" t="s">
+      <c r="D31" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="E31" s="77" t="s">
+      <c r="E31" s="72" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="15"/>
@@ -3952,18 +3953,22 @@
       <c r="BJ31" s="35"/>
       <c r="BK31" s="35"/>
     </row>
-    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B32" s="61"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="56"/>
-      <c r="E32" s="56"/>
+    <row r="32" spans="1:63" s="2" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="49"/>
+      <c r="B32" s="60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="72" t="s">
+        <v>26</v>
+      </c>
       <c r="F32" s="15"/>
-      <c r="G32" s="15" t="str">
+      <c r="G32" s="15" t="e">
         <f t="shared" si="6"/>
-        <v/>
+        <v>#VALUE!</v>
       </c>
       <c r="H32" s="35"/>
       <c r="I32" s="35"/>
@@ -4023,85 +4028,158 @@
       <c r="BK32" s="35"/>
     </row>
     <row r="33" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="B33" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34" t="str">
+      <c r="A33" s="49" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="61"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
-      <c r="AA33" s="37"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
-      <c r="AD33" s="37"/>
-      <c r="AE33" s="37"/>
-      <c r="AF33" s="37"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" s="37"/>
-      <c r="AI33" s="37"/>
-      <c r="AJ33" s="37"/>
-      <c r="AK33" s="37"/>
-      <c r="AL33" s="37"/>
-      <c r="AM33" s="37"/>
-      <c r="AN33" s="37"/>
-      <c r="AO33" s="37"/>
-      <c r="AP33" s="37"/>
-      <c r="AQ33" s="37"/>
-      <c r="AR33" s="37"/>
-      <c r="AS33" s="37"/>
-      <c r="AT33" s="37"/>
-      <c r="AU33" s="37"/>
-      <c r="AV33" s="37"/>
-      <c r="AW33" s="37"/>
-      <c r="AX33" s="37"/>
-      <c r="AY33" s="37"/>
-      <c r="AZ33" s="37"/>
-      <c r="BA33" s="37"/>
-      <c r="BB33" s="37"/>
-      <c r="BC33" s="37"/>
-      <c r="BD33" s="37"/>
-      <c r="BE33" s="37"/>
-      <c r="BF33" s="37"/>
-      <c r="BG33" s="37"/>
-      <c r="BH33" s="37"/>
-      <c r="BI33" s="37"/>
-      <c r="BJ33" s="37"/>
-      <c r="BK33" s="37"/>
-    </row>
-    <row r="34" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F34" s="5"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="35"/>
+      <c r="N33" s="35"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="35"/>
+      <c r="Q33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+      <c r="T33" s="35"/>
+      <c r="U33" s="35"/>
+      <c r="V33" s="35"/>
+      <c r="W33" s="35"/>
+      <c r="X33" s="35"/>
+      <c r="Y33" s="35"/>
+      <c r="Z33" s="35"/>
+      <c r="AA33" s="35"/>
+      <c r="AB33" s="35"/>
+      <c r="AC33" s="35"/>
+      <c r="AD33" s="35"/>
+      <c r="AE33" s="35"/>
+      <c r="AF33" s="35"/>
+      <c r="AG33" s="35"/>
+      <c r="AH33" s="35"/>
+      <c r="AI33" s="35"/>
+      <c r="AJ33" s="35"/>
+      <c r="AK33" s="35"/>
+      <c r="AL33" s="35"/>
+      <c r="AM33" s="35"/>
+      <c r="AN33" s="35"/>
+      <c r="AO33" s="35"/>
+      <c r="AP33" s="35"/>
+      <c r="AQ33" s="35"/>
+      <c r="AR33" s="35"/>
+      <c r="AS33" s="35"/>
+      <c r="AT33" s="35"/>
+      <c r="AU33" s="35"/>
+      <c r="AV33" s="35"/>
+      <c r="AW33" s="35"/>
+      <c r="AX33" s="35"/>
+      <c r="AY33" s="35"/>
+      <c r="AZ33" s="35"/>
+      <c r="BA33" s="35"/>
+      <c r="BB33" s="35"/>
+      <c r="BC33" s="35"/>
+      <c r="BD33" s="35"/>
+      <c r="BE33" s="35"/>
+      <c r="BF33" s="35"/>
+      <c r="BG33" s="35"/>
+      <c r="BH33" s="35"/>
+      <c r="BI33" s="35"/>
+      <c r="BJ33" s="35"/>
+      <c r="BK33" s="35"/>
+    </row>
+    <row r="34" spans="1:63" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="31"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="37"/>
+      <c r="K34" s="37"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="37"/>
+      <c r="R34" s="37"/>
+      <c r="S34" s="37"/>
+      <c r="T34" s="37"/>
+      <c r="U34" s="37"/>
+      <c r="V34" s="37"/>
+      <c r="W34" s="37"/>
+      <c r="X34" s="37"/>
+      <c r="Y34" s="37"/>
+      <c r="Z34" s="37"/>
+      <c r="AA34" s="37"/>
+      <c r="AB34" s="37"/>
+      <c r="AC34" s="37"/>
+      <c r="AD34" s="37"/>
+      <c r="AE34" s="37"/>
+      <c r="AF34" s="37"/>
+      <c r="AG34" s="37"/>
+      <c r="AH34" s="37"/>
+      <c r="AI34" s="37"/>
+      <c r="AJ34" s="37"/>
+      <c r="AK34" s="37"/>
+      <c r="AL34" s="37"/>
+      <c r="AM34" s="37"/>
+      <c r="AN34" s="37"/>
+      <c r="AO34" s="37"/>
+      <c r="AP34" s="37"/>
+      <c r="AQ34" s="37"/>
+      <c r="AR34" s="37"/>
+      <c r="AS34" s="37"/>
+      <c r="AT34" s="37"/>
+      <c r="AU34" s="37"/>
+      <c r="AV34" s="37"/>
+      <c r="AW34" s="37"/>
+      <c r="AX34" s="37"/>
+      <c r="AY34" s="37"/>
+      <c r="AZ34" s="37"/>
+      <c r="BA34" s="37"/>
+      <c r="BB34" s="37"/>
+      <c r="BC34" s="37"/>
+      <c r="BD34" s="37"/>
+      <c r="BE34" s="37"/>
+      <c r="BF34" s="37"/>
+      <c r="BG34" s="37"/>
+      <c r="BH34" s="37"/>
+      <c r="BI34" s="37"/>
+      <c r="BJ34" s="37"/>
+      <c r="BK34" s="37"/>
     </row>
     <row r="35" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="51"/>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:63" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="AJ4:AP4"/>
+    <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
     <mergeCell ref="BE4:BK4"/>
     <mergeCell ref="D3:E3"/>
@@ -4109,11 +4187,8 @@
     <mergeCell ref="O4:U4"/>
     <mergeCell ref="V4:AB4"/>
     <mergeCell ref="AC4:AI4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="AJ4:AP4"/>
-    <mergeCell ref="AQ4:AW4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C33">
+  <conditionalFormatting sqref="C7:C34">
     <cfRule type="dataBar" priority="14">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4127,12 +4202,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BK33">
+  <conditionalFormatting sqref="H5:BK34">
     <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BK33">
+  <conditionalFormatting sqref="H7:BK34">
     <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
@@ -4201,7 +4276,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C33</xm:sqref>
+          <xm:sqref>C7:C34</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>